<commit_message>
ee3dsd: Clock signal analysis
</commit_message>
<xml_diff>
--- a/ee3dsd/cw/cw1/assets/Decoded clocks.xlsx
+++ b/ee3dsd/cw/cw1/assets/Decoded clocks.xlsx
@@ -2554,20 +2554,32 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1000">
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t>Clock</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:rPr lang="en-GB" sz="1000" baseline="0">
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t> signal (s)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB"/>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2592,9 +2604,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2603,7 +2615,7 @@
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2622,16 +2634,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2690,20 +2702,32 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1000">
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t>Arrival</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:rPr lang="en-GB" sz="1000" baseline="0">
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t> time deviation (ms)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB"/>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2728,9 +2752,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2759,16 +2783,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2802,16 +2826,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -3747,13 +3771,17 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t>Clock signal (s)</a:t>
                 </a:r>
               </a:p>
@@ -3780,9 +3808,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -3810,16 +3838,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3878,20 +3906,32 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1000">
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t>Arrival</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:rPr lang="en-GB" sz="1000" baseline="0">
+                    <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                    <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  </a:rPr>
                   <a:t> time (ms)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-GB"/>
+                <a:endParaRPr lang="en-GB" sz="1000">
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3916,9 +3956,9 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -3947,16 +3987,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -5227,12 +5267,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.14344</cdr:x>
+      <cdr:x>0.13076</cdr:x>
       <cdr:y>0.68032</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.89613</cdr:x>
-      <cdr:y>0.68132</cdr:y>
+      <cdr:y>0.68167</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -5241,8 +5281,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="766273" y="2258764"/>
-          <a:ext cx="4021040" cy="3311"/>
+          <a:off x="699685" y="2223384"/>
+          <a:ext cx="4095475" cy="4399"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -5274,12 +5314,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.14467</cdr:x>
+      <cdr:x>0.13076</cdr:x>
       <cdr:y>0.31786</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.89736</cdr:x>
-      <cdr:y>0.31885</cdr:y>
+      <cdr:y>0.31913</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -5288,8 +5328,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="773386" y="1042714"/>
-          <a:ext cx="4023892" cy="3272"/>
+          <a:off x="699685" y="1038794"/>
+          <a:ext cx="4102050" cy="4172"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -5348,6 +5388,11 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-GB" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
@@ -5358,6 +5403,11 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-GB" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
@@ -5367,6 +5417,11 @@
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:endParaRPr lang="en-GB" sz="700">
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
             <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
             <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
             <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
@@ -5468,6 +5523,11 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-GB" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
@@ -5478,6 +5538,11 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-GB" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:latin typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:ea typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               <a:cs typeface="CMU Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
@@ -10121,8 +10186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M58" sqref="M58"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>

</xml_diff>